<commit_message>
Dodávka 07.02.2017, Filip Richter
</commit_message>
<xml_diff>
--- a/board/bom.xlsx
+++ b/board/bom.xlsx
@@ -554,12 +554,6 @@
     <t xml:space="preserve">Distanční sloupek </t>
   </si>
   <si>
-    <t>Objednáno</t>
-  </si>
-  <si>
-    <t>Zbývá</t>
-  </si>
-  <si>
     <t>800-171</t>
   </si>
   <si>
@@ -576,6 +570,12 @@
   </si>
   <si>
     <t>926-LM2596S-5.0/NOPB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na </t>
+  </si>
+  <si>
+    <t>shieldů</t>
   </si>
 </sst>
 </file>
@@ -945,13 +945,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X33"/>
+  <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R2" sqref="R2"/>
+      <selection pane="bottomRight" activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -965,11 +965,10 @@
     <col min="8" max="17" width="0" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="13.44140625"/>
     <col min="19" max="19" width="9" customWidth="1"/>
-    <col min="20" max="20" width="7.77734375" customWidth="1"/>
-    <col min="21" max="1025" width="8.5546875"/>
+    <col min="20" max="1023" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1025,17 +1024,11 @@
       <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1061,28 +1054,17 @@
         <v>25</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="S2">
-        <f t="shared" ref="S2:S33" si="0">IF(C2*7 - R2 &lt; 0, 0, C2*7 - R2)</f>
-        <v>6</v>
-      </c>
-      <c r="T2">
-        <v>6</v>
-      </c>
-      <c r="U2" t="str">
-        <f>IF(S2-T2&gt;0,S2-T2,"")</f>
-        <v/>
-      </c>
-      <c r="V2" t="s">
+        <f>IF(C2*$V$8 - R2 &lt; 0, 0, C2*$V$8 - R2)</f>
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
         <v>26</v>
       </c>
-      <c r="X2">
-        <f>T2+R2</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1108,28 +1090,17 @@
         <v>32</v>
       </c>
       <c r="R3">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="S3">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T3">
-        <v>10</v>
-      </c>
-      <c r="U3" t="str">
-        <f t="shared" ref="U3:U33" si="1">IF(S3-T3&gt;0,S3-T3,"")</f>
-        <v/>
-      </c>
-      <c r="V3" t="s">
+        <f t="shared" ref="S3:S33" si="0">IF(C3*$V$8 - R3 &lt; 0, 0, C3*$V$8 - R3)</f>
+        <v>0</v>
+      </c>
+      <c r="T3" t="s">
         <v>33</v>
       </c>
-      <c r="X3">
-        <f t="shared" ref="X3:X33" si="2">T3+R3</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1155,28 +1126,17 @@
         <v>39</v>
       </c>
       <c r="R4">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="S4">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="T4">
-        <v>10</v>
-      </c>
-      <c r="U4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="V4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T4" t="s">
         <v>40</v>
       </c>
-      <c r="X4">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1202,28 +1162,17 @@
         <v>46</v>
       </c>
       <c r="R5">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="S5">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="T5">
-        <v>7</v>
-      </c>
-      <c r="U5" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="V5" t="s">
+        <v>0</v>
+      </c>
+      <c r="T5" t="s">
         <v>47</v>
       </c>
-      <c r="X5">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1249,28 +1198,17 @@
         <v>39</v>
       </c>
       <c r="R6">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="S6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="T6">
-        <v>10</v>
-      </c>
-      <c r="U6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="V6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T6" t="s">
         <v>51</v>
       </c>
-      <c r="X6">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1296,25 +1234,14 @@
         <v>39</v>
       </c>
       <c r="R7">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="T7">
-        <v>20</v>
-      </c>
-      <c r="U7" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X7">
-        <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1340,25 +1267,23 @@
         <v>32</v>
       </c>
       <c r="R8">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="S8">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="T8">
-        <v>10</v>
-      </c>
-      <c r="U8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X8">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="U8" t="s">
+        <v>181</v>
+      </c>
+      <c r="V8">
+        <v>7</v>
+      </c>
+      <c r="W8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1387,66 +1312,44 @@
         <v>65</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S9">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="T9">
-        <v>10</v>
-      </c>
-      <c r="U9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X9">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>180</v>
-      </c>
       <c r="R10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S10">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="T10">
-        <v>10</v>
-      </c>
-      <c r="U10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X10">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -1481,19 +1384,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X11">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>55</v>
       </c>
@@ -1540,25 +1432,14 @@
         <v>81</v>
       </c>
       <c r="R12">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="S12">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="T12">
-        <v>10</v>
-      </c>
-      <c r="U12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X12">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1584,25 +1465,14 @@
         <v>39</v>
       </c>
       <c r="R13">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="S13">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="T13">
-        <v>10</v>
-      </c>
-      <c r="U13" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X13">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1628,25 +1498,14 @@
         <v>39</v>
       </c>
       <c r="R14">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="S14">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="T14">
-        <v>10</v>
-      </c>
-      <c r="U14" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X14">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1672,25 +1531,14 @@
         <v>39</v>
       </c>
       <c r="R15">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="S15">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="T15">
-        <v>5</v>
-      </c>
-      <c r="U15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X15">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1716,25 +1564,14 @@
         <v>39</v>
       </c>
       <c r="R16">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="S16">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="T16">
-        <v>5</v>
-      </c>
-      <c r="U16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X16">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1760,25 +1597,14 @@
         <v>99</v>
       </c>
       <c r="R17">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="S17">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="T17">
-        <v>5</v>
-      </c>
-      <c r="U17" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X17">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1804,25 +1630,14 @@
         <v>46</v>
       </c>
       <c r="R18">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="S18">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="T18">
-        <v>30</v>
-      </c>
-      <c r="U18" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X18">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
@@ -1851,30 +1666,19 @@
         <v>65</v>
       </c>
       <c r="R19">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S19">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="T19">
-        <v>7</v>
-      </c>
-      <c r="U19" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X19">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1907,25 +1711,14 @@
         <v>118</v>
       </c>
       <c r="R20">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="S20">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="T20">
-        <v>5</v>
-      </c>
-      <c r="U20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X20">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1951,25 +1744,14 @@
         <v>124</v>
       </c>
       <c r="R21">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="S21">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="T21">
-        <v>6</v>
-      </c>
-      <c r="U21" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X21">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -1992,25 +1774,14 @@
         <v>127</v>
       </c>
       <c r="R22">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="S22">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="T22">
-        <v>10</v>
-      </c>
-      <c r="U22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X22">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2036,25 +1807,14 @@
         <v>25</v>
       </c>
       <c r="R23">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="S23">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="T23">
-        <v>10</v>
-      </c>
-      <c r="U23" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X23">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2083,25 +1843,14 @@
         <v>65</v>
       </c>
       <c r="R24">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="S24">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="T24">
-        <v>14</v>
-      </c>
-      <c r="U24" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X24">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -2127,25 +1876,14 @@
         <v>142</v>
       </c>
       <c r="R25">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="S25">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="T25">
-        <v>10</v>
-      </c>
-      <c r="U25" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X25">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -2171,25 +1909,14 @@
         <v>142</v>
       </c>
       <c r="R26">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="S26">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="T26">
-        <v>5</v>
-      </c>
-      <c r="U26" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X26">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2227,25 +1954,14 @@
         <v>152</v>
       </c>
       <c r="R27">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="S27">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="T27">
-        <v>5</v>
-      </c>
-      <c r="U27" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X27">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -2271,25 +1987,14 @@
         <v>46</v>
       </c>
       <c r="R28">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="S28">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T28">
-        <v>3</v>
-      </c>
-      <c r="U28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X28">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
@@ -2318,25 +2023,14 @@
         <v>65</v>
       </c>
       <c r="R29">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S29">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="T29">
-        <v>7</v>
-      </c>
-      <c r="U29" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X29">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>19</v>
       </c>
@@ -2356,25 +2050,14 @@
         <v>165</v>
       </c>
       <c r="R30">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="S30">
         <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="T30">
-        <v>30</v>
-      </c>
-      <c r="U30" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X30">
-        <f t="shared" si="2"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>19</v>
       </c>
@@ -2394,25 +2077,14 @@
         <v>168</v>
       </c>
       <c r="R31">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="S31">
         <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="T31">
-        <v>150</v>
-      </c>
-      <c r="U31" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X31">
-        <f t="shared" si="2"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>19</v>
       </c>
@@ -2432,25 +2104,14 @@
         <v>171</v>
       </c>
       <c r="R32">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="S32">
         <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="T32">
-        <v>23</v>
-      </c>
-      <c r="U32" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X32">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>19</v>
       </c>
@@ -2470,22 +2131,11 @@
         <v>174</v>
       </c>
       <c r="R33">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="S33">
         <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="T33">
-        <v>46</v>
-      </c>
-      <c r="U33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X33">
-        <f t="shared" si="2"/>
-        <v>46</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>